<commit_message>
sepertinya semua permintaan revisi dari tim kampus sudah diperbaiki
</commit_message>
<xml_diff>
--- a/excel/data_tagihan.xlsx
+++ b/excel/data_tagihan.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>bulan</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>ALEXANDER DINGU JAGA MEHA</t>
+  </si>
+  <si>
+    <t>konversi</t>
+  </si>
+  <si>
+    <t>deadline</t>
   </si>
 </sst>
 </file>
@@ -142,7 +148,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -150,34 +156,20 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,11 +485,12 @@
     <col min="1" max="1" width="3.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -508,46 +501,52 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="N1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -557,27 +556,30 @@
       <c r="C2">
         <v>2020</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="4">
+        <v>44104</v>
+      </c>
+      <c r="E2" s="2">
         <v>1216008</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F2">
-        <f>SUM(G2:P2)</f>
+      <c r="G2">
+        <f>SUM(H2:R2)</f>
         <v>1800000</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>850000</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>200000</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>750000</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -587,30 +589,33 @@
       <c r="C3">
         <v>2020</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="4">
+        <v>44104</v>
+      </c>
+      <c r="E3" s="2">
         <v>1216015</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F12" si="0">SUM(G3:P3)</f>
+      <c r="G3">
+        <f t="shared" ref="G3:G12" si="0">SUM(H3:R3)</f>
         <v>1520000</v>
       </c>
-      <c r="G3">
-        <v>500000</v>
-      </c>
       <c r="H3">
+        <v>500000</v>
+      </c>
+      <c r="I3">
         <v>300000</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>700000</v>
       </c>
-      <c r="P3">
+      <c r="R3">
         <v>20000</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -620,33 +625,36 @@
       <c r="C4">
         <v>2020</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="4">
+        <v>44104</v>
+      </c>
+      <c r="E4" s="2">
         <v>1218001</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <f t="shared" si="0"/>
         <v>2260000</v>
       </c>
-      <c r="G4">
-        <v>500000</v>
-      </c>
-      <c r="I4">
+      <c r="H4">
+        <v>500000</v>
+      </c>
+      <c r="J4">
         <v>450000</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>800000</v>
       </c>
-      <c r="O4">
-        <v>500000</v>
-      </c>
       <c r="P4">
+        <v>500000</v>
+      </c>
+      <c r="R4">
         <v>10000</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -656,27 +664,30 @@
       <c r="C5">
         <v>2020</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="4">
+        <v>44104</v>
+      </c>
+      <c r="E5" s="2">
         <v>1218002</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <f t="shared" si="0"/>
         <v>1780000</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>1300000</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>450000</v>
       </c>
-      <c r="P5">
+      <c r="R5">
         <v>30000</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -686,33 +697,36 @@
       <c r="C6">
         <v>2020</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="4">
+        <v>44104</v>
+      </c>
+      <c r="E6" s="2">
         <v>1218003</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <f t="shared" si="0"/>
         <v>1680000</v>
       </c>
-      <c r="G6">
-        <v>500000</v>
-      </c>
       <c r="H6">
         <v>500000</v>
       </c>
       <c r="I6">
+        <v>500000</v>
+      </c>
+      <c r="J6">
         <v>150000</v>
       </c>
-      <c r="O6">
-        <v>500000</v>
-      </c>
       <c r="P6">
+        <v>500000</v>
+      </c>
+      <c r="R6">
         <v>30000</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -722,21 +736,24 @@
       <c r="C7">
         <v>2020</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="4">
+        <v>44104</v>
+      </c>
+      <c r="E7" s="2">
         <v>1218004</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <f t="shared" si="0"/>
         <v>500000</v>
       </c>
-      <c r="O7">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P7">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -746,27 +763,30 @@
       <c r="C8">
         <v>2020</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="4">
+        <v>44104</v>
+      </c>
+      <c r="E8" s="2">
         <v>1218006</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <f t="shared" si="0"/>
         <v>1220000</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>700000</v>
       </c>
-      <c r="O8">
-        <v>500000</v>
-      </c>
       <c r="P8">
+        <v>500000</v>
+      </c>
+      <c r="R8">
         <v>20000</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -776,21 +796,24 @@
       <c r="C9">
         <v>2020</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="4">
+        <v>44104</v>
+      </c>
+      <c r="E9" s="2">
         <v>1218007</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <f t="shared" si="0"/>
         <v>500000</v>
       </c>
-      <c r="O9">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P9">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -800,21 +823,24 @@
       <c r="C10">
         <v>2020</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="4">
+        <v>44104</v>
+      </c>
+      <c r="E10" s="2">
         <v>1218008</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <f t="shared" si="0"/>
         <v>500000</v>
       </c>
-      <c r="O10">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P10">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -824,24 +850,27 @@
       <c r="C11">
         <v>2020</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="4">
+        <v>44104</v>
+      </c>
+      <c r="E11" s="2">
         <v>1218009</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <f t="shared" si="0"/>
         <v>530000</v>
       </c>
-      <c r="O11">
-        <v>500000</v>
-      </c>
       <c r="P11">
+        <v>500000</v>
+      </c>
+      <c r="R11">
         <v>30000</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -851,26 +880,29 @@
       <c r="C12">
         <v>2020</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="4">
+        <v>44104</v>
+      </c>
+      <c r="E12" s="3">
         <v>1219012</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="F12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <f t="shared" si="0"/>
         <v>1350000</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>600000</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>150000</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>550000</v>
       </c>
-      <c r="P12">
+      <c r="R12">
         <v>50000</v>
       </c>
     </row>

</xml_diff>